<commit_message>
CASO DE TESTE COMPLETO
</commit_message>
<xml_diff>
--- a/Caso de Teste - Sistema de Rastreabilidade Agrícola.xlsx
+++ b/Caso de Teste - Sistema de Rastreabilidade Agrícola.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palli\Documents\GitHub\Rastreabilidade_Produtor_Agricola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46BF93A-3B6B-4735-90D1-16DB1AF45F8F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EB248D-86B8-467A-887C-CBB4A936ED33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="15180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="15180" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manter Culturas" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="97">
   <si>
     <t xml:space="preserve">ROTEIRO DE TESTE DE FUNCIONALIDADE DO CASO DE USO </t>
   </si>
@@ -49,12 +49,6 @@
     <t>TOTAL DE ITENS</t>
   </si>
   <si>
-    <t xml:space="preserve">Elaborado por:  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elaborado por: </t>
-  </si>
-  <si>
     <t>Projeto:  Sistema de Rastreabilidade Agrícola</t>
   </si>
   <si>
@@ -70,9 +64,6 @@
     <t>Caso de Uso: Manter Insumos</t>
   </si>
   <si>
-    <t>MANTER INSUMOS</t>
-  </si>
-  <si>
     <t>MANTER CULTURAS</t>
   </si>
   <si>
@@ -104,13 +95,235 @@
   </si>
   <si>
     <t>MANTER VENDAS</t>
+  </si>
+  <si>
+    <t>NOME</t>
+  </si>
+  <si>
+    <t>Entrar com dados exceto String</t>
+  </si>
+  <si>
+    <t>Nome inválido! Digite apenas letras</t>
+  </si>
+  <si>
+    <t>PESQUISA</t>
+  </si>
+  <si>
+    <t>Entrar com caracteres especiais</t>
+  </si>
+  <si>
+    <t>Não digite caracteres especiais!</t>
+  </si>
+  <si>
+    <t>Elaborado por:  Bruno Pallin de Azevedo / William Villela de Caravalho / Daniel Caldeira da Motta</t>
+  </si>
+  <si>
+    <t>COMPOSIÇÃO</t>
+  </si>
+  <si>
+    <t>DOSE</t>
+  </si>
+  <si>
+    <t>CARÊNCIA</t>
+  </si>
+  <si>
+    <t>Entrar com dados exceto números</t>
+  </si>
+  <si>
+    <t>Dose inválida! Digite apenas números</t>
+  </si>
+  <si>
+    <t>Valor inválido!  Insira apenas números</t>
+  </si>
+  <si>
+    <t>Entrar dados com caractéres especiais</t>
+  </si>
+  <si>
+    <t>Composição inválida! Digite apenas letras e números</t>
+  </si>
+  <si>
+    <t>Entrar com dias acima de 28, 29, 30 ou 31</t>
+  </si>
+  <si>
+    <t>Data de pulverização inválida! Digite dias entre 1 e 31</t>
+  </si>
+  <si>
+    <t>DATA (pulverização)</t>
+  </si>
+  <si>
+    <t>Data de pulverizaçao inválida! Digite o mês entre 1 e 12</t>
+  </si>
+  <si>
+    <t>Entrar com mês abaixo de 1 ou acima de 12</t>
+  </si>
+  <si>
+    <t>Entrar com ano acima do atual</t>
+  </si>
+  <si>
+    <t>Data de pulverização inválida! Digite um ano atual ou anterior</t>
+  </si>
+  <si>
+    <t>LOTE</t>
+  </si>
+  <si>
+    <t>DATA (plantio)</t>
+  </si>
+  <si>
+    <t>Data de plantio inválida! Digite um ano atual ou anterior</t>
+  </si>
+  <si>
+    <t>Data de plantio inválida! Digite o mês entre 1 e 12</t>
+  </si>
+  <si>
+    <t>Data de plantio inválida! Digite dias entre 1 e 31</t>
+  </si>
+  <si>
+    <t>DATA (Embalar)</t>
+  </si>
+  <si>
+    <t>Data de embalagem inválida! Digite dias entre 1 e 31</t>
+  </si>
+  <si>
+    <t>Data de embalagem inválida! Digite o mês entre 1 e 12</t>
+  </si>
+  <si>
+    <t>Data de embalagem inválida! Digite um ano atual ou anterior</t>
+  </si>
+  <si>
+    <t>Qnt (Embalar)</t>
+  </si>
+  <si>
+    <t>Quantidade inválida! Digite apenas números</t>
+  </si>
+  <si>
+    <t>CNPJ</t>
+  </si>
+  <si>
+    <t>CCIR</t>
+  </si>
+  <si>
+    <t>NOME DA PROPRIEDADE</t>
+  </si>
+  <si>
+    <t>ENDEREÇO</t>
+  </si>
+  <si>
+    <t>MUNICIPIO</t>
+  </si>
+  <si>
+    <t>UF</t>
+  </si>
+  <si>
+    <t>BAIRRO</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>E-MAIL</t>
+  </si>
+  <si>
+    <t>TEL</t>
+  </si>
+  <si>
+    <t>CNPJ inválido! Digite apenas números</t>
+  </si>
+  <si>
+    <t>Entrar com CCIR inválido</t>
+  </si>
+  <si>
+    <t>CCIR inválido! Digite apenas números</t>
+  </si>
+  <si>
+    <t>Entrar com CNPJ inválido</t>
+  </si>
+  <si>
+    <t>Nome da Propriedade Inválido! Digite apenas letras</t>
+  </si>
+  <si>
+    <t>Nº</t>
+  </si>
+  <si>
+    <t>Endereço inválido! Digite apenas letras</t>
+  </si>
+  <si>
+    <t>Número inválido! Digite apenas números</t>
+  </si>
+  <si>
+    <t>COORDENADAS GEOGRÁFICAS X:</t>
+  </si>
+  <si>
+    <t>COORDENADAS GEOGRÁFICAS Y:</t>
+  </si>
+  <si>
+    <t>Coordenada X inválida! Digite apenas números</t>
+  </si>
+  <si>
+    <t>Entrar com números menores que -180 e maiores que 180</t>
+  </si>
+  <si>
+    <t>Coordenada X inválida! Digite números entre  -180 e 180</t>
+  </si>
+  <si>
+    <t>Município inválido! Digite apenas letras</t>
+  </si>
+  <si>
+    <t>UF inválido! Digite apenas letras</t>
+  </si>
+  <si>
+    <t>Bairro inválido! Digite apenas letras</t>
+  </si>
+  <si>
+    <t>CEP inválido! Digite apenas números</t>
+  </si>
+  <si>
+    <t>Entrar com e-mail inválido</t>
+  </si>
+  <si>
+    <t>E-mail inválido! Digite novamente o e-mail.</t>
+  </si>
+  <si>
+    <t>CNPJ inválido! Digite o CNPJ novamente</t>
+  </si>
+  <si>
+    <t>CCIR inválido! Digite o CCIR novamente</t>
+  </si>
+  <si>
+    <t>Telefone inválido! Digite apenas números</t>
+  </si>
+  <si>
+    <t>NF</t>
+  </si>
+  <si>
+    <t>NF inválida! Digite apenas números</t>
+  </si>
+  <si>
+    <t>DATA (Cadastrar Vendas)</t>
+  </si>
+  <si>
+    <t>Data da venda inválida! Digite o mês entre 1 e 12</t>
+  </si>
+  <si>
+    <t>Data da venda inválida! Digite um ano atual ou anterior</t>
+  </si>
+  <si>
+    <t>Data de venda inválida! Digite dias entre 1 e 31</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>INSC. EST.</t>
+  </si>
+  <si>
+    <t>Insc. Est. inválida! Digite apenas números</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +359,32 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -173,7 +412,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -403,19 +642,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -486,17 +712,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -547,6 +762,100 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -554,7 +863,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -619,28 +928,25 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -649,46 +955,74 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1038,7 +1372,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,7 +1395,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -1070,7 +1404,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="7"/>
@@ -1079,7 +1413,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
@@ -1088,7 +1422,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
@@ -1097,7 +1431,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
@@ -1105,7 +1439,7 @@
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="31" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
@@ -1121,149 +1455,136 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="44" t="s">
-        <v>15</v>
+    <row r="8" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="42" t="s">
+        <v>12</v>
       </c>
       <c r="B8" s="22">
         <v>1</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45"/>
+      <c r="C8" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="43"/>
       <c r="B9" s="22">
         <v>2</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
+      <c r="C9" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45"/>
+      <c r="A10" s="17" t="s">
+        <v>6</v>
+      </c>
       <c r="B10" s="22">
-        <v>3</v>
-      </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="18">
-        <v>4</v>
-      </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="44"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+    </row>
+    <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
-      <c r="B12" s="20">
-        <v>5</v>
-      </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="45"/>
-      <c r="B13" s="19">
-        <v>6</v>
-      </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="45"/>
-      <c r="B14" s="28">
-        <v>7</v>
-      </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="31"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="45"/>
-      <c r="B15" s="22">
-        <v>8</v>
-      </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="45"/>
-      <c r="B16" s="22">
-        <v>9</v>
-      </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="45"/>
-      <c r="B17" s="28">
-        <v>10</v>
-      </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="45"/>
-      <c r="B18" s="28">
-        <v>11</v>
-      </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="45"/>
-      <c r="B19" s="22">
-        <v>12</v>
-      </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="45"/>
-      <c r="B20" s="22">
-        <v>13</v>
-      </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="45"/>
-      <c r="B21" s="22">
-        <v>14</v>
-      </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="9">
-        <v>14</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="40"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="40"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="A8:A21"/>
+  <mergeCells count="1">
+    <mergeCell ref="A8:A9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1272,10 +1593,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C608BF8C-8C35-434E-9123-1C07D9935799}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="A1:E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,7 +1619,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -1307,7 +1628,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="7"/>
@@ -1316,7 +1637,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
@@ -1325,7 +1646,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
@@ -1334,7 +1655,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
@@ -1342,7 +1663,7 @@
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="31" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
@@ -1358,148 +1679,141 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
-        <v>14</v>
+    <row r="8" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="42" t="s">
+        <v>12</v>
       </c>
       <c r="B8" s="22">
         <v>1</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
+      <c r="C8" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="47"/>
       <c r="B9" s="22">
         <v>2</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39"/>
+      <c r="C9" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="47"/>
       <c r="B10" s="22">
         <v>3</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
+      <c r="C10" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="47"/>
       <c r="B11" s="18">
         <v>4</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="20">
+      <c r="C11" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="47"/>
+      <c r="B12" s="54">
         <v>5</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39"/>
-      <c r="B13" s="19">
+      <c r="C12" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="47"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="43"/>
+      <c r="B15" s="22">
+        <v>5</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
-      <c r="B14" s="28">
-        <v>7</v>
-      </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="31"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
-      <c r="B15" s="22">
-        <v>8</v>
-      </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
-      <c r="B16" s="22">
-        <v>9</v>
-      </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="39"/>
-      <c r="B17" s="28">
-        <v>10</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
-      <c r="B18" s="28">
-        <v>11</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
-      <c r="B19" s="22">
-        <v>12</v>
-      </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39"/>
-      <c r="B20" s="22">
-        <v>13</v>
-      </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
-      <c r="B21" s="22">
-        <v>14</v>
-      </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="9">
-        <v>14</v>
-      </c>
+      <c r="B16" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="11"/>
     </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="41"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A8:A21"/>
+  <mergeCells count="3">
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="B12:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1507,10 +1821,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1382E0C7-BD1A-49BE-9600-55754E3E7CC3}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,7 +1847,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -1542,7 +1856,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="7"/>
@@ -1551,7 +1865,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
@@ -1560,7 +1874,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
@@ -1569,7 +1883,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
@@ -1577,7 +1891,7 @@
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="31" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
@@ -1593,149 +1907,89 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="44" t="s">
-        <v>16</v>
+    <row r="8" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="35" t="s">
+        <v>13</v>
       </c>
       <c r="B8" s="22">
         <v>1</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45"/>
+      <c r="C8" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="36"/>
       <c r="B9" s="22">
         <v>2</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
+      <c r="C9" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>27</v>
+      </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45"/>
-      <c r="B10" s="22">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="36"/>
+      <c r="B10" s="50">
         <v>3</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="18">
-        <v>4</v>
-      </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
-      <c r="B12" s="20">
-        <v>5</v>
-      </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
+      <c r="C10" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="36"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="37"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="45"/>
+      <c r="A13" s="17" t="s">
+        <v>6</v>
+      </c>
       <c r="B13" s="19">
-        <v>6</v>
-      </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="45"/>
-      <c r="B14" s="28">
-        <v>7</v>
-      </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="31"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="45"/>
-      <c r="B15" s="22">
-        <v>8</v>
-      </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="45"/>
-      <c r="B16" s="22">
-        <v>9</v>
-      </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="45"/>
-      <c r="B17" s="28">
-        <v>10</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="45"/>
-      <c r="B18" s="28">
-        <v>11</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="45"/>
-      <c r="B19" s="22">
-        <v>12</v>
-      </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="45"/>
-      <c r="B20" s="22">
-        <v>13</v>
-      </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="45"/>
-      <c r="B21" s="22">
-        <v>14</v>
-      </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="9">
-        <v>14</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A8:A21"/>
-    <mergeCell ref="C11:C13"/>
+  <mergeCells count="3">
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B10:B12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1743,10 +1997,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADAA937-90B3-4CFA-8364-3F5AE9BFDE25}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,7 +2008,7 @@
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1769,7 +2023,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -1778,7 +2032,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="7"/>
@@ -1787,7 +2041,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
@@ -1796,7 +2050,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
@@ -1805,7 +2059,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
@@ -1813,7 +2067,7 @@
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="31" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
@@ -1829,149 +2083,88 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="44" t="s">
-        <v>19</v>
+    <row r="8" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="42" t="s">
+        <v>16</v>
       </c>
       <c r="B8" s="22">
         <v>1</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45"/>
-      <c r="B9" s="22">
+      <c r="C8" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="47"/>
+      <c r="B9" s="50">
         <v>2</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45"/>
-      <c r="B10" s="22">
+      <c r="C9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="47"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="47"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="43"/>
+      <c r="B12" s="20">
         <v>3</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="18">
-        <v>4</v>
-      </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
-      <c r="B12" s="20">
-        <v>5</v>
-      </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
+      <c r="C12" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="45"/>
+      <c r="A13" s="17" t="s">
+        <v>6</v>
+      </c>
       <c r="B13" s="19">
-        <v>6</v>
-      </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="45"/>
-      <c r="B14" s="28">
-        <v>7</v>
-      </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="31"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="45"/>
-      <c r="B15" s="22">
-        <v>8</v>
-      </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="45"/>
-      <c r="B16" s="22">
-        <v>9</v>
-      </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="45"/>
-      <c r="B17" s="28">
-        <v>10</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="45"/>
-      <c r="B18" s="28">
-        <v>11</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="45"/>
-      <c r="B19" s="22">
-        <v>12</v>
-      </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="45"/>
-      <c r="B20" s="22">
-        <v>13</v>
-      </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="45"/>
-      <c r="B21" s="22">
-        <v>14</v>
-      </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="9">
-        <v>14</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A8:A21"/>
-    <mergeCell ref="C11:C13"/>
+  <mergeCells count="3">
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B9:B11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1979,22 +2172,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A0E436-BC66-49CF-8A34-55B4C0E7E9DF}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2003,53 +2196,53 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="7"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
@@ -2065,159 +2258,313 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
-        <v>21</v>
+    <row r="8" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="42" t="s">
+        <v>18</v>
       </c>
       <c r="B8" s="22">
         <v>1</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
+      <c r="C8" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="47"/>
       <c r="B9" s="22">
         <v>2</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39"/>
-      <c r="B10" s="22">
+      <c r="C9" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="47"/>
+      <c r="B10" s="50">
         <v>3</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="18">
+      <c r="C10" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="47"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="47"/>
+      <c r="B12" s="50">
         <v>4</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="20">
+      <c r="C12" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="41"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="47"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="47"/>
+      <c r="B14" s="20">
         <v>5</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39"/>
-      <c r="B13" s="19">
+      <c r="C14" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="47"/>
+      <c r="B15" s="19">
         <v>6</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
-      <c r="B14" s="28">
+      <c r="C15" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="47"/>
+      <c r="B16" s="28">
         <v>7</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="31"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
-      <c r="B15" s="22">
+      <c r="C16" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="47"/>
+      <c r="B17" s="50">
         <v>8</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
-      <c r="B16" s="22">
+      <c r="C17" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="47"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="47"/>
+      <c r="B19" s="50">
         <v>9</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="39"/>
-      <c r="B17" s="28">
+      <c r="C19" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="47"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="47"/>
+      <c r="B21" s="22">
         <v>10</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
-      <c r="B18" s="28">
+      <c r="C21" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="47"/>
+      <c r="B22" s="22">
         <v>11</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
-      <c r="B19" s="22">
+      <c r="C22" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="47"/>
+      <c r="B23" s="22">
         <v>12</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39"/>
-      <c r="B20" s="22">
+      <c r="C23" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="47"/>
+      <c r="B24" s="22">
         <v>13</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
-      <c r="B21" s="22">
+      <c r="C24" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="47"/>
+      <c r="B25" s="22">
         <v>14</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
+      <c r="C25" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="43"/>
+      <c r="B26" s="22">
+        <v>15</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="9">
-        <v>14</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
+      <c r="B27" s="22">
+        <v>15</v>
+      </c>
+      <c r="E27" s="41"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A8:A21"/>
+  <mergeCells count="9">
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="A8:A26"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A03597E-29F4-4CEA-A77C-4A2E0539A76D}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2240,7 +2587,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -2249,7 +2596,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="7"/>
@@ -2258,7 +2605,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
@@ -2267,7 +2614,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
@@ -2276,7 +2623,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
@@ -2284,7 +2631,7 @@
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="31" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
@@ -2300,148 +2647,91 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
-        <v>25</v>
+    <row r="8" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="42" t="s">
+        <v>22</v>
       </c>
       <c r="B8" s="22">
         <v>1</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
+      <c r="C8" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="47"/>
       <c r="B9" s="22">
         <v>2</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39"/>
-      <c r="B10" s="22">
+      <c r="C9" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="47"/>
+      <c r="B10" s="50">
         <v>3</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="18">
-        <v>4</v>
-      </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="20">
-        <v>5</v>
-      </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
+      <c r="C10" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="47"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="43"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39"/>
+      <c r="A13" s="17" t="s">
+        <v>6</v>
+      </c>
       <c r="B13" s="19">
-        <v>6</v>
-      </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
-      <c r="B14" s="28">
-        <v>7</v>
-      </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="31"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
-      <c r="B15" s="22">
-        <v>8</v>
-      </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
-      <c r="B16" s="22">
-        <v>9</v>
-      </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="39"/>
-      <c r="B17" s="28">
-        <v>10</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
-      <c r="B18" s="28">
-        <v>11</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
-      <c r="B19" s="22">
-        <v>12</v>
-      </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39"/>
-      <c r="B20" s="22">
-        <v>13</v>
-      </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
-      <c r="B21" s="22">
-        <v>14</v>
-      </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="9">
-        <v>14</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L17" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A8:A21"/>
+  <mergeCells count="3">
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A8:A12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2449,10 +2739,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1EF20C9-E558-40DC-A777-51FC098A7C4C}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2475,7 +2765,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -2484,7 +2774,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="7"/>
@@ -2493,7 +2783,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
@@ -2502,7 +2792,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
@@ -2511,7 +2801,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
@@ -2519,7 +2809,7 @@
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="31" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
@@ -2535,148 +2825,137 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
-        <v>24</v>
+    <row r="8" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="42" t="s">
+        <v>21</v>
       </c>
       <c r="B8" s="22">
         <v>1</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
-      <c r="B9" s="22">
+      <c r="C8" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="47"/>
+      <c r="B9" s="50">
         <v>2</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39"/>
-      <c r="B10" s="22">
+      <c r="C9" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="47"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="47"/>
+      <c r="B11" s="20">
         <v>3</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="18">
+      <c r="C11" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="47"/>
+      <c r="B12" s="19">
         <v>4</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="20">
+      <c r="C12" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="47"/>
+      <c r="B13" s="28">
         <v>5</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39"/>
-      <c r="B13" s="19">
+      <c r="C13" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="47"/>
+      <c r="B14" s="22">
         <v>6</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
-      <c r="B14" s="28">
+      <c r="C14" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="43"/>
+      <c r="B15" s="22">
         <v>7</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="31"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
-      <c r="B15" s="22">
-        <v>8</v>
-      </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
+      <c r="C15" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
-      <c r="B16" s="22">
-        <v>9</v>
-      </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="39"/>
-      <c r="B17" s="28">
-        <v>10</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
-      <c r="B18" s="28">
-        <v>11</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
-      <c r="B19" s="22">
-        <v>12</v>
-      </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39"/>
-      <c r="B20" s="22">
-        <v>13</v>
-      </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
-      <c r="B21" s="22">
-        <v>14</v>
-      </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
+      <c r="A16" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="9">
-        <v>14</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
+      <c r="B16" s="56">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A8:A21"/>
+  <mergeCells count="3">
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A8:A15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>